<commit_message>
work on conditional formatting
</commit_message>
<xml_diff>
--- a/src/main/resources/avmeldewesen/avmeldewesen.xlsx
+++ b/src/main/resources/avmeldewesen/avmeldewesen.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/sources/dox43/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\H$\sources\dox43\src\main\resources\avmeldewesen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE450D5-387E-E14C-9D5E-94D066F230AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="4160" windowWidth="30240" windowHeight="18360" activeTab="1" xr2:uid="{6CCFD295-1CCF-445D-9327-8EE5976927A7}"/>
+    <workbookView xWindow="5400" yWindow="4155" windowWidth="8670" windowHeight="9690" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Grundstücke" sheetId="1" r:id="rId1"/>
-    <sheet name="Gebäude" sheetId="2" r:id="rId2"/>
+    <sheet name="Grundstücke-if" sheetId="3" r:id="rId2"/>
+    <sheet name="Gebäude" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,13 +37,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Marcus Warm</author>
     <author>Stefan Ziegler</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B08E0DB6-23A3-4D66-8C49-1BFB8FD2C639}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{85FB8EC2-020B-489D-8CD0-3B8E6E806A19}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="1" shapeId="0" xr:uid="{413D0EDE-7260-B141-9542-DA90251D2558}">
+    <comment ref="A14" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -145,12 +145,75 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Marcus Warm</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jxlsteam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:area(lastCell="C2" sheetStreaming="false")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jxlsteam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="grundstuecke" var="m" lastCell="C2")
+jx:if(condition="m['flaechenmass']&lt;1000" lastCell="C2" areas=["A2:C2", "A3:C3"])</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Stefan Ziegler</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{9DA562EF-A87D-2A46-99C2-175B0C82D32F}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -164,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{3D718639-5D9D-834A-A0CE-2D650AA77965}">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -183,7 +246,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
   <si>
     <t>${m['nummer']}</t>
   </si>
@@ -225,12 +288,15 @@
   </si>
   <si>
     <t>${singlevalue}</t>
+  </si>
+  <si>
+    <t>qqqq</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -292,7 +358,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,6 +383,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -332,7 +404,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -347,26 +419,28 @@
     <xf numFmtId="3" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% - Accent6" xfId="2" builtinId="50"/>
-    <cellStyle name="60% - Accent5" xfId="1" builtinId="48"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="20 % - Akzent6" xfId="2" builtinId="50"/>
+    <cellStyle name="60 % - Akzent5" xfId="1" builtinId="48"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="0" xr9:uid="{9A2F7AC3-10FC-BB40-A0CC-C718257721B7}"/>
+    <tableStyle name="Table Style 1" pivot="0" count="0"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -675,19 +749,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139056DA-F565-48DD-A2AA-3D287E85F6DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="142" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -697,8 +771,11 @@
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -709,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -719,7 +796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -727,10 +804,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>1000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -738,19 +820,83 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3328B787-C282-B04F-AF2E-6800BF1B6AF7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7">
+        <f>SUM(C2)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView zoomScale="141" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="17.1640625" customWidth="1"/>
+    <col min="1" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>7</v>
       </c>
@@ -761,7 +907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
wip on xls formatting
</commit_message>
<xml_diff>
--- a/src/main/resources/avmeldewesen/avmeldewesen.xlsx
+++ b/src/main/resources/avmeldewesen/avmeldewesen.xlsx
@@ -172,7 +172,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="C2" sheetStreaming="false")</t>
+jx:area(lastCell="C4" sheetStreaming="false")
+</t>
         </r>
       </text>
     </comment>
@@ -198,8 +199,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="grundstuecke" var="m" lastCell="C2")
-jx:if(condition="m['flaechenmass']&lt;1000" lastCell="C2" areas=["A2:C2", "A3:C3"])</t>
+jx:each(items="grundstuecke" var="m" lastCell="C3")
+jx:if(condition="m['flaechenmass']&lt;1000" lastCell="C3" areas=["A2:C2", "A3:C3"])</t>
         </r>
       </text>
     </comment>
@@ -246,7 +247,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>${m['nummer']}</t>
   </si>
@@ -291,6 +292,9 @@
   </si>
   <si>
     <t>qqqq</t>
+  </si>
+  <si>
+    <t>fff</t>
   </si>
 </sst>
 </file>
@@ -821,10 +825,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +838,7 @@
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -844,8 +848,11 @@
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -856,7 +863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -867,13 +874,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7">
-        <f>SUM(C2)</f>
+        <f>SUM(C2:C3)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>